<commit_message>
Working version of the tool
</commit_message>
<xml_diff>
--- a/Tank and composite data.xlsx
+++ b/Tank and composite data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan Struzinski\Documents\DARE\Sparrow - feed\Netting theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB133D8-1C5F-4EEF-88CF-9118C8B4E205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC106FE-FC34-4803-9D42-555D8610039B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8AEA6481-0AB0-4E25-B197-3D5CC263106A}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{8AEA6481-0AB0-4E25-B197-3D5CC263106A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E50B84-5329-44DE-B885-3FF352A99BD9}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +535,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>180.8</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -620,7 +620,7 @@
         <v>28</v>
       </c>
       <c r="B15">
-        <v>0.25</v>
+        <v>0.27500000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>